<commit_message>
Cards changes. Hound, Ogre, Tomb, Shopkeeper. Did I just commit them?
</commit_message>
<xml_diff>
--- a/sheet/EventCardData.xlsx
+++ b/sheet/EventCardData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAAA728-608B-4BF4-8FBF-146C2B92C9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47BF5F6-FEF1-434E-BF7D-304849AAF61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -248,11 +248,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>多选：①可重复 支付1金币为1张道具牌充1能。②支付3金币，从遗物牌堆翻开3张牌，选其中1张获得。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1任意属性，10时间：升1级。使用1张《智力》发动本牌时，可以少消耗2时间。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多选：①可重复 支付1金币为1张道具牌充1能。②支付3金币，从遗物牌堆翻开3张牌，选其中1张获得。③可重复 弃置1张任意战利品牌，获得1金币。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -755,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Changed some cards to test structure deck.
</commit_message>
<xml_diff>
--- a/sheet/EventCardData.xlsx
+++ b/sheet/EventCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47BF5F6-FEF1-434E-BF7D-304849AAF61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F84DDE-A989-49CF-9F28-FE16561C66C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,39 +220,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2时间：将主牌堆第1张怪物牌放在房间区任意非空列顶端，然后获得遭遇牌堆第1张战利品牌，再获得遗物牌堆顶的1张遗物牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1任意属性/1时间：重抽房间区所有牌。使用1张《感知》发动本牌时，可以再重抽任意张手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1任意属性/1时间：选1张位于房间区最前方的怪物牌横置。使用1张《敏捷》发动本牌时，可以再选1张位于房间区最前方的怪物牌横置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1任意属性/1时间：将房间区最前方任意1张牌移动到战场敌人列第一行。使用1张《敏捷》发动本牌时，可以将房间区任意1张牌移动到战场敌人列第一行。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1任意属性/1时间：获得遭遇牌堆第1张战利品牌。使用1张《感知》发动本牌时，转而翻开遭遇牌堆前3张战利品牌中选1张获得。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1任意属性/1时间：选房间区1张陷阱牌移动到房间区任意位置。使用1张《感知》发动本牌时，可以转而选弃牌堆1张陷阱牌放到房间区任意位置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1任意属性/1时间：从遭遇牌堆翻开3张牌，获得其中的战利品牌。使用1张《敏捷》发动本牌时，可以额外翻开2张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1任意属性，10时间：升1级。使用1张《智力》发动本牌时，可以少消耗2时间。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>多选：①可重复 支付1金币为1张道具牌充1能。②支付3金币，从遗物牌堆翻开3张牌，选其中1张获得。③可重复 弃置1张任意战利品牌，获得1金币。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用1任意属性，或将1张手牌洗回主牌堆：重抽房间区所有牌。使用1张《感知》发动本牌时，可以再重抽任意张手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用1任意属性，或将1张手牌洗回主牌堆：选1张位于房间区最前方的怪物牌横置。使用1张《敏捷》发动本牌时，可以再选1张位于房间区最前方的怪物牌横置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用1任意属性，或将1张手牌洗回主牌堆：将房间区最前方任意1张牌移动到战场敌人列第一行。使用1张《敏捷》发动本牌时，可以将房间区任意1张牌移动到战场敌人列第一行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用1任意属性，或将1张手牌洗回主牌堆：获得遭遇牌堆第1张战利品牌。使用1张《感知》发动本牌时，转而翻开遭遇牌堆前3张战利品牌中选1张获得。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用1任意属性，或将1张手牌洗回主牌堆：选房间区1张陷阱牌移动到房间区任意位置。使用1张《感知》发动本牌时，可以转而选弃牌堆1张陷阱牌放到房间区任意位置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用1任意属性，或将1张手牌洗回主牌堆：从遭遇牌堆翻开3张牌，获得其中的战利品牌。使用1张《敏捷》发动本牌时，可以额外翻开2张牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗2时间：将主牌堆第1张怪物牌放在房间区任意非空列顶端，然后获得遭遇牌堆第1张战利品牌，再获得遗物牌堆顶的1张遗物牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗10时间，然后使用1任意属性或将1张手牌洗回主牌堆：升1级。使用1张《智力》发动本牌时，可以少消耗2时间。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -683,7 +683,7 @@
       <c r="E4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -738,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -755,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Card changes. 1. Now with Mimic Tooth the player can place at most 1 card in the opponent side for each row. 2. Add cost for Wine Glass. 3. Trainer now cost 3 time units and 1 attribute/hand card instead of 5 time units. 4. The shopkeeper now discard 1 loot card for 1 GP. 5. The Trade machine now has all its effect being optional. 6. Sludge now kills all cards with rank 1 instead of only slime cards.
</commit_message>
<xml_diff>
--- a/sheet/EventCardData.xlsx
+++ b/sheet/EventCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F87404-1013-4F65-AAB4-25B4046A450D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF9E038-328F-4971-AE3E-F45606467388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,22 +220,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>消耗2时间：将主牌堆第1张怪物牌放在房间区任意非空列顶端，然后获得遭遇牌堆第1张战利品牌，再获得遗物牌堆顶的1张遗物牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>祭坛</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>将1张手牌送墓，或弃置1张战利品牌，或受到1点伤害：获得1道具点。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>消耗5时间，然后使用1任意属性或将1张手牌洗回主牌堆：获得1技能点。使用1张《智力》发动本牌时，可以少消耗2时间。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>消耗1时间，或使用1任意属性，或将1张手牌洗回主牌堆：重抽房间区所有牌。使用1张《感知》发动本牌时，可以再重抽任意张手牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -256,11 +244,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>消耗1时间，或使用1任意属性，或将1张手牌洗回主牌堆：从遭遇牌堆翻开3张牌，获得其中的战利品牌。使用1张《敏捷》发动本牌时，可以额外翻开2张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多选，可重复：①支付1金币，获得1道具点。②支付2道具点，获得1金币。②支付3金币，从遗物牌堆翻开3张牌，选其中1张获得。</t>
+    <t>多选，可重复：①支付1金币，获得1道具点。②弃置1张战利品牌，获得1金币。③支付3金币，从遗物牌堆翻开3张牌，选其中1张获得。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗3时间，然后使用1任意属性或将1张手牌洗回主牌堆：获得1技能点。使用1张《智力》发动本牌时，可以少消耗2时间。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗2时间，然后使用1任意属性或将1张手牌洗回主牌堆：将主牌堆第1张怪物牌放在房间区任意非空列顶端，然后获得遭遇牌堆第1张战利品牌，再获得遗物牌堆顶的1张遗物牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将1张手牌送墓，或弃置1张战利品牌，或受到1点伤害：获得1道具点，或获得遭遇牌堆第1张战利品牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗1时间，或使用1任意属性，或将1张手牌洗回主牌堆：从遭遇牌堆翻开5张牌，获得其中的战利品牌。使用1张《敏捷》发动本牌时，可以额外翻开2张牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,7 +613,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -656,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -673,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2"/>
       <c r="G3" s="2"/>
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2"/>
       <c r="G4" s="2"/>
@@ -699,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2"/>
       <c r="G5" s="2"/>
@@ -712,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -729,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
@@ -746,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -780,7 +780,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
@@ -791,13 +791,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the effects of most cards, making them relevant to the new change in rules. Added some alternative version of existing trap cards.
</commit_message>
<xml_diff>
--- a/sheet/EventCardData.xlsx
+++ b/sheet/EventCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E199E93-5D0A-4525-A80A-8B5ABC821394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541BF89-6BA1-42ED-9E4C-01AB7B2A7512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -245,23 +245,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>从遭遇牌堆翻开5张牌，获得其中的战利品牌。使用1张《敏捷》发动本牌时，可以额外翻开2张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>重抽房间区所有牌。横置1张“体质”牌，可以再重抽任意张手牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>消耗3时间，将主牌堆第1张怪物牌放在房间区任意空槽位，然后获得遭遇牌堆第1张战利品牌，再获得遗物牌堆顶的1张遗物牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>消耗2时间，获得1SP。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>多选：①将1张手牌送墓，翻开遭遇牌堆顶1张牌，如果是战利品牌则可以获得。②弃置1张战利品牌，获得1道具点。③受到3伤害，获得1SP。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得遭遇牌堆第1张战利品牌。使用1张《敏捷》发动本牌时，可以再获得1张战利品牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗3时间，将主牌堆第1张怪物牌放在房间区任意空槽位，然后获得遭遇牌堆第1张战利品牌，再获得遗物牌堆第1张遗物牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -730,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
@@ -747,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
@@ -781,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>18</v>
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Goo's card effect. It now get -1 to its rank every time it splits.
</commit_message>
<xml_diff>
--- a/sheet/EventCardData.xlsx
+++ b/sheet/EventCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541BF89-6BA1-42ED-9E4C-01AB7B2A7512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372F1AA1-E88F-4B8D-BD7F-414BA4016C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>cardName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tags</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>宝箱</t>
   </si>
   <si>
@@ -57,10 +53,6 @@
   </si>
   <si>
     <t>cardNameEn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tagsEn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -611,194 +603,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="32.125" customWidth="1"/>
-    <col min="7" max="7" width="62.5" customWidth="1"/>
+    <col min="3" max="3" width="32.125" customWidth="1"/>
+    <col min="5" max="5" width="62.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="92.25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2">
+      <c r="B11">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="92.25" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamings. Some cards are removed due to previous rule change. Some card descriptions are changed due to previous rule change.
</commit_message>
<xml_diff>
--- a/sheet/EventCardData.xlsx
+++ b/sheet/EventCardData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92E33D2-4149-4E2F-9F4D-F2B4B8C6C02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FE32D7-BC11-45F7-9980-E083FD672A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="2910" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>cardName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>宝箱</t>
-  </si>
-  <si>
-    <t>拉杆</t>
-  </si>
-  <si>
-    <t>冒险者尸体</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cardNameEn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -68,15 +58,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dead adventurer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Resource merchant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>训练师</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -160,35 +142,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>① Activate only when there is any non-empty column in the Exploration Zone: Add the first three { Loot } cards from the Event Deck to your Loot Zone. Then add the first { Monster } card from the Main Deck to the top of any non-empty column in the Exploration Zone.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>① Activate, repeatable: Trade 2 non-gold resource for 1 gold or trade 1 gold for 1 non-gold resource. &lt;br&gt;
 ② Activate only when the Player does not have [Wanted] artifact card: Get 1 resource of each type. Then add a [Wanted] card from the Artifact Deck to your Equipment Zone.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Trainer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>① Activate only when there are more than 10 cards in the Graveyard: Send 10 cards in the Graveyard back to the Main Deck and get 1 Attribute Token.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>杂物堆</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>拐角</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>maxCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -209,51 +171,52 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>多选，可重复：①支付1金币，获得1道具点。②弃置1张战利品牌，获得1金币。③支付3金币，从遗物牌堆翻开3张牌，选其中1张获得。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>房间出口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>隐蔽处</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选房间区1张怪物牌横置。横置1张“敏捷”牌，可以改为选房间区任意怪物牌横置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选场上1张怪物牌移动到其同区域内的一个空槽位中。横置1张“敏捷”牌，可以改为交换场上两个同区域槽位的所有牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>翻开遭遇牌堆前3张牌，获得其中1张战利品牌。横置1张“感知”牌，可以改为翻开遭遇牌堆前5张牌，获得其中所有战利品牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选场上1张陷阱牌，将其移动到场上任意位置或送墓。横置1张“智力”牌，可以改为将弃牌堆顶端的1张陷阱牌移动到场上任意位置或送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重抽房间区所有牌。横置1张“体质”牌，可以再重抽任意张手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>消耗2时间，获得1SP。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得遭遇牌堆第1张战利品牌。使用1张《敏捷》发动本牌时，可以再获得1张战利品牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>消耗3时间，将主牌堆第1张怪物牌放在房间区任意空槽位，然后获得遭遇牌堆第1张战利品牌，再获得遗物牌堆第1张遗物牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多选：①将1张手牌送墓，翻开遭遇牌堆顶1张牌，如果是战利品牌则可以获得。②弃置1张战利品牌，获得1道具点。③受到2伤害，获得1SP。</t>
+    <t>地下城重整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重抽场上所有敌人侧的牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>翻开遭遇牌堆前3张牌，获得其中1张物品牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉杆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选场上1张陷阱牌，触发它或将其移动到场上任意位置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得遭遇牌堆第1张物品牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宝箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商店</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多选：①可重复，弃置1张物品牌，然后获得1金币。②取遭遇牌堆前3张物品牌，然后玩家每支付2金币，可以获得其中1张牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多选：①弃置1张物品牌。②将1张手牌送墓。③受到2伤害。&lt;br&gt;
+执行2项以上时：从购买能力区选1张牌获得。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>训练场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可重复：支付3金币，从购买能力区选1张牌获得。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -603,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -620,171 +583,122 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="92.25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="92.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add repeat limit to Merchant card's selling item effect. Add reroll effect to Trainer card.
</commit_message>
<xml_diff>
--- a/sheet/EventCardData.xlsx
+++ b/sheet/EventCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED9DDC3-2C28-4160-BE3F-2874500367CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD5B52-5C1A-4DB9-B317-F10A71526DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,10 +203,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>多选：①可重复，弃置1张物品牌，然后获得1金币。②取遭遇牌堆前3张物品牌，然后玩家每支付2金币，可以获得其中1张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>多选：①弃置1张物品牌。②将1张手牌送墓。③受到2伤害。&lt;br&gt;
 执行2项以上时：从购买能力区选1张牌获得。</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -216,15 +212,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>可重复：支付3金币，从购买能力区选1张牌获得。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>足迹</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>将弃牌堆顶的1张牌放回主牌堆。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多选：①可重复至多3次，弃置1张物品牌，然后获得1金币。②取遭遇牌堆前3张物品牌，然后玩家每支付2金币，可以获得其中1张牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多选：①可重复，支付3金币，从购买能力区选1张牌获得。②可重复至多3次，支付1金币，将购买能力区补满，然后重抽其中任意张牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -577,7 +577,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -672,13 +672,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -691,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
@@ -702,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
@@ -711,15 +711,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>